<commit_message>
Requests Ioanna, 2 April. Untested.
</commit_message>
<xml_diff>
--- a/Participation in education and training (excluding guided on the job training).xlsx
+++ b/Participation in education and training (excluding guided on the job training).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\0_LLL\1.LFS-E\8. LFS adult learning\Final evaluation\GOTJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eceuropaeu-my.sharepoint.com/personal/aleksander_rutkowski_ec_europa_eu/Documents/Social_Scoreboard_in_R/FRESH NEW APPROACH/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7D8049-C284-4815-85C2-8ABC30281060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="21549" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'ISCED - 2016'!$A:$A</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'ISCED - 2022'!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1418,140 +1418,140 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="219.42578125" style="75" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="74"/>
+    <col min="1" max="1" width="219.3828125" style="75" customWidth="1"/>
+    <col min="2" max="16384" width="9.15234375" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="73" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="75" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="75" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="79" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="76" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="76" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="76" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="77" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="76" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="80.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="76" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="79" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="10" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="76"/>
     </row>
-    <row r="13" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="73" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="76" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="80" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="80" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="80" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="80" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="80" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="75" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="75" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="75" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="78" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="79" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="40" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="78" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A27" s="81"/>
     </row>
   </sheetData>
@@ -1584,14 +1584,14 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="4" customWidth="1"/>
-    <col min="2" max="7" width="10.7109375" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="7" width="10.69140625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -1599,7 +1599,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="38.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="82" t="s">
         <v>1</v>
@@ -1620,7 +1620,7 @@
       <c r="F4" s="82"/>
       <c r="G4" s="82"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="7" t="s">
         <v>3</v>
@@ -1641,7 +1641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>40.700000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>52.6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>47.1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>46.7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>51.3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>44.8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>42.7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>51.8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>54.4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>27</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>28</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>29</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>30</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>43.6</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>31</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>57.3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>33</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>55.6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="59" t="s">
         <v>73</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>74</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>75</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>36</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>71</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="64" t="s">
         <v>76</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="67" t="s">
         <v>62</v>
       </c>
@@ -2492,14 +2492,14 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="4" customWidth="1"/>
-    <col min="2" max="7" width="10.7109375" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="13.15234375" style="4" customWidth="1"/>
+    <col min="2" max="7" width="10.69140625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -2507,7 +2507,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -2515,7 +2515,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="38.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32"/>
       <c r="B4" s="82" t="s">
         <v>1</v>
@@ -2528,7 +2528,7 @@
       <c r="F4" s="82"/>
       <c r="G4" s="82"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="7" t="s">
         <v>3</v>
@@ -2549,7 +2549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>6</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>38.799999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>47.1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>54.7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>50.7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>53.4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>27</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>28</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>29</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>30</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>31</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>57.7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>33</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>34</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>36</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>71</v>
       </c>
@@ -3285,12 +3285,12 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A39" s="30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:D4"/>
@@ -3309,24 +3309,24 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="4" customWidth="1"/>
-    <col min="2" max="11" width="10.7109375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="20.3828125" style="4" customWidth="1"/>
+    <col min="2" max="11" width="10.69140625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="82" t="s">
         <v>39</v>
@@ -3343,7 +3343,7 @@
       <c r="J4" s="82"/>
       <c r="K4" s="82"/>
     </row>
-    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="24.9" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="31" t="s">
         <v>41</v>
@@ -3376,7 +3376,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>27</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>28</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>77</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>30</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>31</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>33</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>42.7</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>51.4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="59" t="s">
         <v>73</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>74</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>78</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>36</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>71</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="59" t="s">
         <v>76</v>
       </c>
@@ -4636,12 +4636,12 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A44" s="67" t="s">
         <v>62</v>
       </c>
@@ -4664,24 +4664,24 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="4" customWidth="1"/>
-    <col min="2" max="11" width="10.7109375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="13.3046875" style="4" customWidth="1"/>
+    <col min="2" max="11" width="10.69140625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="82" t="s">
         <v>39</v>
@@ -4698,7 +4698,7 @@
       <c r="J4" s="82"/>
       <c r="K4" s="82"/>
     </row>
-    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="24.9" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="31" t="s">
         <v>41</v>
@@ -4731,7 +4731,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>64</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>44.8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>39.799999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>27</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>28</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>29</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>30</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>31</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>33</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>55.7</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>34</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>36</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>71</v>
       </c>
@@ -5851,12 +5851,12 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A40" s="30" t="s">
         <v>62</v>
       </c>
@@ -5875,18 +5875,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E597368F-2B70-4BCC-A003-2BF8C83EC61F}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
-    <col min="2" max="9" width="20.7109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="22.53515625" style="4" customWidth="1"/>
+    <col min="2" max="9" width="20.69140625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -5895,7 +5895,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -5904,7 +5904,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32"/>
       <c r="B4" s="82" t="s">
         <v>39</v>
@@ -5919,7 +5919,7 @@
       <c r="H4" s="82"/>
       <c r="I4" s="82"/>
     </row>
-    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="49.75" x14ac:dyDescent="0.3">
       <c r="A5" s="68"/>
       <c r="B5" s="31" t="s">
         <v>47</v>
@@ -5946,7 +5946,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>58.1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>59.2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>52</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>66.900000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>62.1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>53</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>49.6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>69.3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>80</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>56.2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>60.8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>59.2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>27</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>28</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>63.8</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>77</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>30</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>31</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>33</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>70.3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>79.7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="59" t="s">
         <v>73</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>60.1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>81</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>82</v>
       </c>
@@ -6903,7 +6903,7 @@
         <v>26.3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>36</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
         <v>71</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="59" t="s">
         <v>83</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>54</v>
       </c>
@@ -6999,7 +6999,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>55</v>
       </c>
@@ -7008,7 +7008,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A45" s="67" t="s">
         <v>62</v>
       </c>
@@ -7038,14 +7038,14 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="4" customWidth="1"/>
-    <col min="2" max="9" width="20.7109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="13.53515625" style="4" customWidth="1"/>
+    <col min="2" max="9" width="20.69140625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
@@ -7054,7 +7054,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -7063,7 +7063,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32"/>
       <c r="B4" s="82" t="s">
         <v>39</v>
@@ -7078,7 +7078,7 @@
       <c r="H4" s="82"/>
       <c r="I4" s="82"/>
     </row>
-    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="49.75" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="31" t="s">
         <v>47</v>
@@ -7105,7 +7105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>52</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>66</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>53</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>51.3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>60.2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>67</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>54.7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>41.8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -7627,7 +7627,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>68</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>28</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>29</v>
       </c>
@@ -7801,7 +7801,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>69</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>48.1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>70</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>33</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>34</v>
       </c>
@@ -7946,7 +7946,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>36</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>71</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>54</v>
       </c>
@@ -8042,7 +8042,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
@@ -8051,7 +8051,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A41" s="30" t="s">
         <v>62</v>
       </c>
@@ -8060,7 +8060,7 @@
       <c r="D41" s="30"/>
       <c r="E41" s="30"/>
     </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:E4"/>
@@ -8082,25 +8082,25 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="4" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="1.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="4" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="2.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="13.3828125" style="4" customWidth="1"/>
+    <col min="2" max="3" width="10.69140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="1.69140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.69140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="1.69140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.69140625" style="4" customWidth="1"/>
+    <col min="9" max="10" width="10.69140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="1.69140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.69140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="1.69140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="10.69140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="2.69140625" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="9.15234375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -8117,7 +8117,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
@@ -8134,7 +8134,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32"/>
       <c r="B4" s="82" t="s">
         <v>1</v>
@@ -8155,7 +8155,7 @@
       <c r="N4" s="82"/>
       <c r="O4" s="82"/>
     </row>
-    <row r="5" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="7">
         <v>2007</v>
@@ -8188,7 +8188,7 @@
       </c>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>6</v>
       </c>
@@ -8233,7 +8233,7 @@
       </c>
       <c r="O6" s="38"/>
     </row>
-    <row r="7" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
@@ -8276,7 +8276,7 @@
       </c>
       <c r="O7" s="28"/>
     </row>
-    <row r="8" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -8319,7 +8319,7 @@
       </c>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -8362,7 +8362,7 @@
       </c>
       <c r="O9" s="16"/>
     </row>
-    <row r="10" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -8405,7 +8405,7 @@
       </c>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -8448,7 +8448,7 @@
       </c>
       <c r="O11" s="16"/>
     </row>
-    <row r="12" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -8491,7 +8491,7 @@
       </c>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
@@ -8534,7 +8534,7 @@
       </c>
       <c r="O13" s="16"/>
     </row>
-    <row r="14" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
@@ -8577,7 +8577,7 @@
       </c>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
@@ -8620,7 +8620,7 @@
       </c>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>16</v>
       </c>
@@ -8667,7 +8667,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -8710,7 +8710,7 @@
       </c>
       <c r="O17" s="16"/>
     </row>
-    <row r="18" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>18</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -8798,7 +8798,7 @@
       </c>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>20</v>
       </c>
@@ -8841,7 +8841,7 @@
       </c>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
@@ -8884,7 +8884,7 @@
       </c>
       <c r="O21" s="16"/>
     </row>
-    <row r="22" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
@@ -8927,7 +8927,7 @@
       </c>
       <c r="O22" s="16"/>
     </row>
-    <row r="23" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -8972,7 +8972,7 @@
       </c>
       <c r="O23" s="16"/>
     </row>
-    <row r="24" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -9015,7 +9015,7 @@
       </c>
       <c r="O24" s="16"/>
     </row>
-    <row r="25" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
@@ -9058,7 +9058,7 @@
       </c>
       <c r="O25" s="16"/>
     </row>
-    <row r="26" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
@@ -9101,7 +9101,7 @@
       </c>
       <c r="O26" s="16"/>
     </row>
-    <row r="27" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>27</v>
       </c>
@@ -9144,7 +9144,7 @@
       </c>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>28</v>
       </c>
@@ -9187,7 +9187,7 @@
       </c>
       <c r="O28" s="16"/>
     </row>
-    <row r="29" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>29</v>
       </c>
@@ -9232,7 +9232,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>30</v>
       </c>
@@ -9275,7 +9275,7 @@
       </c>
       <c r="O30" s="16"/>
     </row>
-    <row r="31" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>31</v>
       </c>
@@ -9318,7 +9318,7 @@
       </c>
       <c r="O31" s="16"/>
     </row>
-    <row r="32" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
@@ -9361,7 +9361,7 @@
       </c>
       <c r="O32" s="19"/>
     </row>
-    <row r="33" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>33</v>
       </c>
@@ -9404,7 +9404,7 @@
       </c>
       <c r="O33" s="22"/>
     </row>
-    <row r="34" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>34</v>
       </c>
@@ -9447,7 +9447,7 @@
       </c>
       <c r="O34" s="25"/>
     </row>
-    <row r="35" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>35</v>
       </c>
@@ -9490,7 +9490,7 @@
       </c>
       <c r="O35" s="22"/>
     </row>
-    <row r="36" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>36</v>
       </c>
@@ -9531,7 +9531,7 @@
       </c>
       <c r="O36" s="25"/>
     </row>
-    <row r="37" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>71</v>
       </c>
@@ -9572,7 +9572,7 @@
       </c>
       <c r="O37" s="22"/>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="30" t="s">
         <v>62</v>
       </c>

</xml_diff>